<commit_message>
Update of GINF1 Modules
</commit_message>
<xml_diff>
--- a/resources/GINF1/modules.xlsx
+++ b/resources/GINF1/modules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\AP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55EF1FE-CDD7-4DCC-82C2-D60955CDB4C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58DE23A-D6CA-4853-AA31-06135118508E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5115" yWindow="2760" windowWidth="15375" windowHeight="8325" xr2:uid="{4C56605D-1814-484D-BD67-6BFC85BD123D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Code</t>
   </si>
@@ -37,6 +37,144 @@
   </si>
   <si>
     <t>Chef  Module</t>
+  </si>
+  <si>
+    <t>GINF11</t>
+  </si>
+  <si>
+    <t>GINF12</t>
+  </si>
+  <si>
+    <t>GINF13</t>
+  </si>
+  <si>
+    <t>GINF14</t>
+  </si>
+  <si>
+    <t>GINF15</t>
+  </si>
+  <si>
+    <t>GINF16</t>
+  </si>
+  <si>
+    <t>GINF21</t>
+  </si>
+  <si>
+    <t>GINF22</t>
+  </si>
+  <si>
+    <t>GINF23</t>
+  </si>
+  <si>
+    <t>GINF24</t>
+  </si>
+  <si>
+    <t>GINF25</t>
+  </si>
+  <si>
+    <t>GINF26</t>
+  </si>
+  <si>
+    <t>Maths pour l'ingénieur</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>Electronique 1</t>
+  </si>
+  <si>
+    <t>Programmation</t>
+  </si>
+  <si>
+    <t>BD &amp; Réseaux</t>
+  </si>
+  <si>
+    <t>Langues et Communication</t>
+  </si>
+  <si>
+    <t>Développement Informatique</t>
+  </si>
+  <si>
+    <t>BD : Développemenent et Manipulation</t>
+  </si>
+  <si>
+    <t>Théories des Graphes et recherches opérationnelle</t>
+  </si>
+  <si>
+    <t>Réseaux 1</t>
+  </si>
+  <si>
+    <t>Architectures et Linux</t>
+  </si>
+  <si>
+    <t>Management de l'entreprise 1</t>
+  </si>
+  <si>
+    <t>Siham</t>
+  </si>
+  <si>
+    <t>El Oualkadi</t>
+  </si>
+  <si>
+    <t>Amechnoue</t>
+  </si>
+  <si>
+    <t>Tanana</t>
+  </si>
+  <si>
+    <t>Haris</t>
+  </si>
+  <si>
+    <t>El Haddad</t>
+  </si>
+  <si>
+    <t>Fissoune Rachida</t>
+  </si>
+  <si>
+    <t>Samadi</t>
+  </si>
+  <si>
+    <t>Belmokadem</t>
+  </si>
+  <si>
+    <t>NAIT BOUKER Nezha</t>
+  </si>
+  <si>
+    <t>Traitement de Signal</t>
+  </si>
+  <si>
+    <t>Electronique analogique, Electronique numérique</t>
+  </si>
+  <si>
+    <t>C, Programmation web PHP</t>
+  </si>
+  <si>
+    <t>BD relationnelle, Concept fondamentaux des réseaux</t>
+  </si>
+  <si>
+    <t>Développement personnel</t>
+  </si>
+  <si>
+    <t>POO C++,Programmation Web PHP5 &amp; Mysql</t>
+  </si>
+  <si>
+    <t>Méthodes et modélisation BD, PLSQL</t>
+  </si>
+  <si>
+    <t>Recherche Opérationnel, Théorie des graphes</t>
+  </si>
+  <si>
+    <t>Protocole et Adressage réseaux, Technologie des réseaux, TP CISCO</t>
+  </si>
+  <si>
+    <t>Micro-Achitecture des processeur, Assembleur, Linux</t>
+  </si>
+  <si>
+    <t>Gestion des entreprises, Comptabilité, Economie</t>
+  </si>
+  <si>
+    <t>Statistiques</t>
   </si>
 </sst>
 </file>
@@ -388,16 +526,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9078595-6E23-491B-9A56-4D7BC37B86BD}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -414,6 +553,171 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>